<commit_message>
finished fix bugs of sltu and sltiu of CPU
</commit_message>
<xml_diff>
--- a/ControlUnit.xlsx
+++ b/ControlUnit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programming\BUAA_CO_2020\cscore\P3_SingleCycleCPU\pre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D81BE2F-11A7-4BB0-9583-37C72CBD70C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF3A93A-103B-4149-B2E1-C3A372291C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9672" yWindow="888" windowWidth="19872" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1667,20 +1667,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1696,9 +1684,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1763,8 +1748,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2048,2295 +2048,2264 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41:N48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="10" style="9" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="8"/>
-    <col min="5" max="5" width="10.77734375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="9"/>
-    <col min="9" max="9" width="11.6640625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="6.109375" style="10" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="8" style="9" customWidth="1"/>
-    <col min="14" max="15" width="6.88671875" style="28" customWidth="1"/>
-    <col min="16" max="16" width="9" style="28" customWidth="1"/>
-    <col min="17" max="17" width="6.88671875" style="10" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" style="9" customWidth="1"/>
-    <col min="19" max="19" width="10.77734375" style="10" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" style="9" customWidth="1"/>
-    <col min="21" max="21" width="6.77734375" style="9" customWidth="1"/>
-    <col min="22" max="22" width="7.44140625" style="10" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="10" style="5" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="10.77734375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="11.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="8" style="5" customWidth="1"/>
+    <col min="14" max="15" width="6.88671875" style="23" customWidth="1"/>
+    <col min="16" max="16" width="9" style="23" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="7.33203125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" style="6" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" style="5" customWidth="1"/>
+    <col min="21" max="21" width="6.77734375" style="5" customWidth="1"/>
+    <col min="22" max="22" width="7.44140625" style="6" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="9" t="s">
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="29" t="s">
+      <c r="O4" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="P4" s="29" t="s">
+      <c r="P4" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="S4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="T4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="20" t="s">
+      <c r="U4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="V4" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:22" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="20">
         <v>0</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="20">
         <v>0</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="20">
         <v>0</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="22">
         <v>0</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="25" t="s">
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="S5" s="27"/>
-      <c r="T5" s="25" t="s">
+      <c r="S5" s="22"/>
+      <c r="T5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="U5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="V5" s="27" t="s">
+      <c r="V5" s="22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="5"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="2"/>
     </row>
     <row r="7" spans="1:22" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="O7" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="P7" s="33" t="s">
+      <c r="P7" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="R7" s="8"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="5"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="2"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="8" t="s">
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="5"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="2"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8" t="s">
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="5"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8" t="s">
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="5"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="8" t="s">
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="5"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="8" t="s">
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="5"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8" t="s">
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="5"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="8" t="s">
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="5"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="8" t="s">
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="5"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="8" t="s">
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="5"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F17" s="22"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="5"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="5"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="2"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M19" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="N19" s="33" t="s">
+      <c r="N19" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="O19" s="33" t="s">
+      <c r="O19" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="P19" s="31" t="s">
+      <c r="P19" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="Q19" s="7" t="s">
+      <c r="Q19" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="R19" s="8"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="5"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="2"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="31" t="s">
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="5"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="2"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="31" t="s">
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="5"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="2"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="31" t="s">
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="Q22" s="7" t="s">
+      <c r="Q22" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="R22" s="8"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="5"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="2"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="31" t="s">
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="5"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="31" t="s">
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="5"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="2"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F25" s="22"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="5"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="2"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F26" s="22"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="5"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="2"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="5"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="2"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="K28" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="L28" s="8" t="s">
+      <c r="L28" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M28" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="N28" s="31" t="s">
+      <c r="N28" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O28" s="33" t="s">
+      <c r="O28" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="P28" s="33" t="s">
+      <c r="P28" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="Q28" s="7" t="s">
+      <c r="Q28" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="R28" s="8"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="5"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="2"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="8" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M29" s="1"/>
-      <c r="N29" s="31" t="s">
+      <c r="M29" s="33"/>
+      <c r="N29" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="5"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="2"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="9" t="s">
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="31" t="s">
+      <c r="M30" s="33"/>
+      <c r="N30" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="7"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="29"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="8" t="s">
+      <c r="F31" s="32"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="M31" s="1"/>
-      <c r="N31" s="31" t="s">
+      <c r="M31" s="33"/>
+      <c r="N31" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="5"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="2"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="8" t="s">
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M32" s="1"/>
-      <c r="N32" s="31" t="s">
+      <c r="M32" s="33"/>
+      <c r="N32" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="5"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="2"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="8" t="s">
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="M33" s="1"/>
-      <c r="N33" s="31" t="s">
+      <c r="M33" s="33"/>
+      <c r="N33" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="5"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="8" t="s">
+      <c r="F34" s="32"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="31" t="s">
+      <c r="M34" s="33"/>
+      <c r="N34" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O34" s="33"/>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="5"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="2"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="9" t="s">
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="M35" s="1"/>
-      <c r="N35" s="31" t="s">
+      <c r="M35" s="33"/>
+      <c r="N35" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O35" s="33"/>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="7"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="29"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F37" s="22"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="31"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="5"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="2"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F38" s="22"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
-      <c r="P38" s="31"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="5"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="2"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F39" s="22"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="31"/>
-      <c r="P39" s="31"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="5"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="31"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="5"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="2"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="I41" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="J41" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="K41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="L41" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="M41" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="N41" s="33" t="s">
+      <c r="N41" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="O41" s="33" t="s">
+      <c r="O41" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="P41" s="32" t="s">
+      <c r="P41" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="Q41" s="6" t="s">
+      <c r="Q41" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="R41" s="8"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="5"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="2"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F42" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I42" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J42" s="8" t="s">
+      <c r="J42" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L42" s="4"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="5"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="27"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="2"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="F43" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I43" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="J43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K43" s="5" t="s">
+      <c r="K43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L43" s="4"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="33"/>
-      <c r="O43" s="33"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="5"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="28"/>
+      <c r="O43" s="28"/>
+      <c r="P43" s="27"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="2"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="22" t="s">
+      <c r="F44" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="K44" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L44" s="4"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="32"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="8"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="5"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="28"/>
+      <c r="P44" s="27"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="2"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G45" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H45" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I45" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J45" s="8" t="s">
+      <c r="J45" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K45" s="5" t="s">
+      <c r="K45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L45" s="4"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="33"/>
-      <c r="O45" s="33"/>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="5"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F46" s="22" t="s">
+      <c r="F46" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G46" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H46" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="I46" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="J46" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K46" s="5" t="s">
+      <c r="K46" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L46" s="4"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="33"/>
-      <c r="O46" s="33"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="8"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="8"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="5"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="2"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="I47" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J47" s="8" t="s">
+      <c r="J47" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L47" s="4"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="8"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="5"/>
+      <c r="L47" s="32"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="28"/>
+      <c r="P47" s="27"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="2"/>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F48" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I48" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="J48" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K48" s="5" t="s">
+      <c r="K48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="4"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="33"/>
-      <c r="O48" s="33"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="8"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="5"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="28"/>
+      <c r="P48" s="27"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="2"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="22"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="31"/>
-      <c r="O49" s="31"/>
-      <c r="P49" s="31"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="5"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="2"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="F50" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="H50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="I50" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="J50" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K50" s="5" t="s">
+      <c r="K50" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L50" s="8" t="s">
+      <c r="L50" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M50" s="8"/>
-      <c r="N50" s="31" t="s">
+      <c r="M50" s="4"/>
+      <c r="N50" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="O50" s="33" t="s">
+      <c r="O50" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="P50" s="31"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="8" t="s">
+      <c r="P50" s="26"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U50" s="8" t="s">
+      <c r="U50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="V50" s="5" t="s">
+      <c r="V50" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F51" s="22" t="s">
+      <c r="F51" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="I51" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J51" s="8" t="s">
+      <c r="J51" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K51" s="5" t="s">
+      <c r="K51" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L51" s="8" t="s">
+      <c r="L51" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M51" s="8"/>
-      <c r="N51" s="31" t="s">
+      <c r="M51" s="4"/>
+      <c r="N51" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="O51" s="33"/>
-      <c r="P51" s="31"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="8"/>
-      <c r="S51" s="5"/>
-      <c r="T51" s="8" t="s">
+      <c r="O51" s="28"/>
+      <c r="P51" s="26"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U51" s="8" t="s">
+      <c r="U51" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="V51" s="5" t="s">
+      <c r="V51" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F52" s="22" t="s">
+      <c r="F52" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="I52" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J52" s="8" t="s">
+      <c r="J52" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K52" s="5" t="s">
+      <c r="K52" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L52" s="8" t="s">
+      <c r="L52" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M52" s="8"/>
-      <c r="N52" s="31" t="s">
+      <c r="M52" s="4"/>
+      <c r="N52" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="O52" s="33"/>
-      <c r="P52" s="31"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="8"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="8" t="s">
+      <c r="O52" s="28"/>
+      <c r="P52" s="26"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U52" s="8" t="s">
+      <c r="U52" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="V52" s="5" t="s">
+      <c r="V52" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="22" t="s">
+      <c r="F53" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H53" s="8" t="s">
+      <c r="H53" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="I53" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="J53" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K53" s="5" t="s">
+      <c r="K53" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L53" s="8" t="s">
+      <c r="L53" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M53" s="8"/>
-      <c r="N53" s="31" t="s">
+      <c r="M53" s="4"/>
+      <c r="N53" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="O53" s="33"/>
-      <c r="P53" s="31"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="8"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="8" t="s">
+      <c r="O53" s="28"/>
+      <c r="P53" s="26"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U53" s="8" t="s">
+      <c r="U53" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="V53" s="5" t="s">
+      <c r="V53" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F54" s="22"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="31"/>
-      <c r="O54" s="31"/>
-      <c r="P54" s="31"/>
-      <c r="Q54" s="5"/>
-      <c r="R54" s="8"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="8"/>
-      <c r="U54" s="8"/>
-      <c r="V54" s="5"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="2"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G55" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="I55" s="8"/>
-      <c r="J55" s="1" t="s">
+      <c r="I55" s="4"/>
+      <c r="J55" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="K55" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="L55" s="4" t="s">
+      <c r="L55" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="M55" s="8" t="s">
+      <c r="M55" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N55" s="31" t="s">
+      <c r="N55" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="O55" s="33" t="s">
+      <c r="O55" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="P55" s="31"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="8" t="s">
+      <c r="P55" s="26"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S55" s="5" t="s">
+      <c r="S55" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="T55" s="8"/>
-      <c r="U55" s="8"/>
-      <c r="V55" s="5"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="2"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="8" t="s">
+      <c r="F56" s="32"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="29"/>
+      <c r="L56" s="32"/>
+      <c r="M56" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="N56" s="31" t="s">
+      <c r="N56" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O56" s="33"/>
-      <c r="P56" s="31"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="8" t="s">
+      <c r="O56" s="28"/>
+      <c r="P56" s="26"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S56" s="24" t="s">
+      <c r="S56" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="T56" s="8"/>
-      <c r="U56" s="8"/>
-      <c r="V56" s="5"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="2"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F57" s="4"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="8" t="s">
+      <c r="F57" s="32"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="29"/>
+      <c r="L57" s="32"/>
+      <c r="M57" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="N57" s="31" t="s">
+      <c r="N57" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="O57" s="33"/>
-      <c r="P57" s="31"/>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="8" t="s">
+      <c r="O57" s="28"/>
+      <c r="P57" s="26"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S57" s="5" t="s">
+      <c r="S57" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="T57" s="8"/>
-      <c r="U57" s="8"/>
-      <c r="V57" s="5"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="2"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E58" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="8" t="s">
+      <c r="F58" s="32"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="29"/>
+      <c r="L58" s="32"/>
+      <c r="M58" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="N58" s="31" t="s">
+      <c r="N58" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="O58" s="33"/>
-      <c r="P58" s="31"/>
-      <c r="Q58" s="5"/>
-      <c r="R58" s="8" t="s">
+      <c r="O58" s="28"/>
+      <c r="P58" s="26"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S58" s="5" t="s">
+      <c r="S58" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="T58" s="8"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="5"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="2"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F59" s="4"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="8" t="s">
+      <c r="F59" s="32"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="29"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="N59" s="31" t="s">
+      <c r="N59" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O59" s="33"/>
-      <c r="P59" s="31"/>
-      <c r="Q59" s="5"/>
-      <c r="R59" s="8" t="s">
+      <c r="O59" s="28"/>
+      <c r="P59" s="26"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S59" s="24" t="s">
+      <c r="S59" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="T59" s="8"/>
-      <c r="U59" s="8"/>
-      <c r="V59" s="5"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="2"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F60" s="4"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="8" t="s">
+      <c r="F60" s="32"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N60" s="31" t="s">
+      <c r="N60" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="O60" s="33"/>
-      <c r="P60" s="31"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="8" t="s">
+      <c r="O60" s="28"/>
+      <c r="P60" s="26"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S60" s="5" t="s">
+      <c r="S60" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="T60" s="8"/>
-      <c r="U60" s="8"/>
-      <c r="V60" s="5"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="2"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="5" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="O28:O35"/>
-    <mergeCell ref="P28:P35"/>
-    <mergeCell ref="Q28:Q35"/>
-    <mergeCell ref="O55:O60"/>
-    <mergeCell ref="O41:O48"/>
-    <mergeCell ref="O50:O53"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="O7:O16"/>
-    <mergeCell ref="P7:P16"/>
-    <mergeCell ref="Q7:Q16"/>
-    <mergeCell ref="L19:L24"/>
-    <mergeCell ref="M19:M24"/>
-    <mergeCell ref="N19:N24"/>
-    <mergeCell ref="O19:O24"/>
-    <mergeCell ref="Q19:Q21"/>
-    <mergeCell ref="Q22:Q24"/>
-    <mergeCell ref="F19:F24"/>
-    <mergeCell ref="G19:G24"/>
-    <mergeCell ref="H19:H24"/>
-    <mergeCell ref="I19:I24"/>
-    <mergeCell ref="J19:J24"/>
-    <mergeCell ref="K28:K35"/>
-    <mergeCell ref="N7:N16"/>
-    <mergeCell ref="L41:L48"/>
-    <mergeCell ref="L55:L60"/>
-    <mergeCell ref="M7:M16"/>
-    <mergeCell ref="M28:M35"/>
-    <mergeCell ref="N41:N48"/>
-    <mergeCell ref="K19:K24"/>
-    <mergeCell ref="F55:F60"/>
-    <mergeCell ref="G55:G60"/>
-    <mergeCell ref="H55:H60"/>
-    <mergeCell ref="J55:J60"/>
-    <mergeCell ref="K55:K60"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="M41:M48"/>
@@ -4351,6 +4320,40 @@
     <mergeCell ref="H28:H35"/>
     <mergeCell ref="I28:I35"/>
     <mergeCell ref="J28:J35"/>
+    <mergeCell ref="F55:F60"/>
+    <mergeCell ref="G55:G60"/>
+    <mergeCell ref="H55:H60"/>
+    <mergeCell ref="J55:J60"/>
+    <mergeCell ref="K55:K60"/>
+    <mergeCell ref="K28:K35"/>
+    <mergeCell ref="N7:N16"/>
+    <mergeCell ref="L41:L48"/>
+    <mergeCell ref="L55:L60"/>
+    <mergeCell ref="M7:M16"/>
+    <mergeCell ref="M28:M35"/>
+    <mergeCell ref="N41:N48"/>
+    <mergeCell ref="K19:K24"/>
+    <mergeCell ref="F19:F24"/>
+    <mergeCell ref="G19:G24"/>
+    <mergeCell ref="H19:H24"/>
+    <mergeCell ref="I19:I24"/>
+    <mergeCell ref="J19:J24"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="O7:O16"/>
+    <mergeCell ref="P7:P16"/>
+    <mergeCell ref="Q7:Q16"/>
+    <mergeCell ref="L19:L24"/>
+    <mergeCell ref="M19:M24"/>
+    <mergeCell ref="N19:N24"/>
+    <mergeCell ref="O19:O24"/>
+    <mergeCell ref="Q19:Q21"/>
+    <mergeCell ref="Q22:Q24"/>
+    <mergeCell ref="O28:O35"/>
+    <mergeCell ref="P28:P35"/>
+    <mergeCell ref="Q28:Q35"/>
+    <mergeCell ref="O55:O60"/>
+    <mergeCell ref="O41:O48"/>
+    <mergeCell ref="O50:O53"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>